<commit_message>
refined conceptual model for 0b default
</commit_message>
<xml_diff>
--- a/default/0b - year_filters/concept.xlsx
+++ b/default/0b - year_filters/concept.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Documents\GitHub\pyesm\default\0b - year_filters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19D5BD7B-6A7C-4E4B-9B8B-7554C0E65D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B9A6A50-D1E0-4510-A926-B9626EB96094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13890" yWindow="0" windowWidth="24615" windowHeight="15585" xr2:uid="{E114F217-1283-47A9-999D-63924FD6D4FE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E114F217-1283-47A9-999D-63924FD6D4FE}"/>
   </bookViews>
   <sheets>
     <sheet name="concept" sheetId="2" r:id="rId1"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -680,7 +680,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -727,16 +727,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="4" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="4" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -756,11 +754,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1053,13 +1049,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BE05235-892E-456B-BF7F-0596A6B82F2A}">
-  <dimension ref="A1:AQ48"/>
+  <dimension ref="A1:AQ47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="9" ySplit="10" topLeftCell="J11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="Z27" sqref="Z27"/>
+      <selection pane="bottomRight" activeCell="Q12" sqref="Q12:S13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1089,7 +1085,7 @@
       <c r="A1" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="48"/>
+      <c r="B1" s="45"/>
       <c r="C1" s="19"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -1174,11 +1170,11 @@
       </c>
     </row>
     <row r="2" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A2" s="50"/>
-      <c r="B2" s="51" t="s">
+      <c r="A2" s="47"/>
+      <c r="B2" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="52"/>
+      <c r="C2" s="48"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -1263,7 +1259,7 @@
     </row>
     <row r="3" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A3" s="20"/>
-      <c r="B3" s="49"/>
+      <c r="B3" s="46"/>
       <c r="C3" s="21" t="s">
         <v>57</v>
       </c>
@@ -1353,7 +1349,7 @@
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
-      <c r="D4" s="55" t="s">
+      <c r="D4" s="51" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="2"/>
@@ -1405,7 +1401,7 @@
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="56" t="s">
+      <c r="D5" s="52" t="s">
         <v>74</v>
       </c>
       <c r="E5" s="2"/>
@@ -1457,22 +1453,19 @@
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
-      <c r="D6" s="57" t="s">
+      <c r="D6" s="53" t="s">
         <v>68</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
-      <c r="K6" s="47" t="s">
+      <c r="K6" t="s">
         <v>63</v>
       </c>
-      <c r="L6" s="47"/>
-      <c r="M6" s="47"/>
-      <c r="N6" s="47" t="s">
+      <c r="N6" t="s">
         <v>64</v>
       </c>
-      <c r="O6" s="47"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
@@ -1556,10 +1549,10 @@
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="58" t="s">
+      <c r="F8" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="G8" s="59" t="s">
+      <c r="G8" s="55" t="s">
         <v>73</v>
       </c>
       <c r="H8" s="2"/>
@@ -1607,19 +1600,19 @@
         <v>4</v>
       </c>
       <c r="I9" s="2"/>
-      <c r="K9" s="32" t="s">
+      <c r="K9" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="L9" s="32" t="s">
+      <c r="L9" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="M9" s="32" t="s">
+      <c r="M9" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="N9" s="32" t="s">
+      <c r="N9" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="O9" s="32" t="s">
+      <c r="O9" s="30" t="s">
         <v>81</v>
       </c>
       <c r="P9" s="4"/>
@@ -1776,7 +1769,6 @@
       <c r="AA12" s="22">
         <v>15</v>
       </c>
-      <c r="AB12" s="27"/>
       <c r="AC12" s="23" cm="1">
         <f t="array" ref="AC12:AI13">MMULT($K$12:$O$13,TRANSPOSE($K23:$O29))</f>
         <v>30</v>
@@ -1799,27 +1791,26 @@
       <c r="AI12" s="23">
         <v>15</v>
       </c>
-      <c r="AJ12" s="27"/>
-      <c r="AK12" s="33" cm="1">
+      <c r="AK12" s="31" cm="1">
         <f t="array" ref="AK12:AQ13">_xlfn.ANCHORARRAY(AC12)-U$12:AA$13</f>
         <v>0</v>
       </c>
-      <c r="AL12" s="35">
+      <c r="AL12" s="33">
         <v>2.9999999995311555E-7</v>
       </c>
-      <c r="AM12" s="36">
-        <v>0</v>
-      </c>
-      <c r="AN12" s="36">
-        <v>0</v>
-      </c>
-      <c r="AO12" s="36">
-        <v>0</v>
-      </c>
-      <c r="AP12" s="36">
-        <v>0</v>
-      </c>
-      <c r="AQ12" s="37">
+      <c r="AM12" s="34">
+        <v>0</v>
+      </c>
+      <c r="AN12" s="34">
+        <v>0</v>
+      </c>
+      <c r="AO12" s="34">
+        <v>0</v>
+      </c>
+      <c r="AP12" s="34">
+        <v>0</v>
+      </c>
+      <c r="AQ12" s="35">
         <v>0</v>
       </c>
     </row>
@@ -1872,7 +1863,6 @@
       <c r="AA13" s="22">
         <v>150</v>
       </c>
-      <c r="AB13" s="27"/>
       <c r="AC13" s="23">
         <v>0</v>
       </c>
@@ -1894,26 +1884,25 @@
       <c r="AI13" s="23">
         <v>150</v>
       </c>
-      <c r="AJ13" s="27"/>
-      <c r="AK13" s="34">
-        <v>0</v>
-      </c>
-      <c r="AL13" s="38">
-        <v>0</v>
-      </c>
-      <c r="AM13" s="39">
-        <v>0</v>
-      </c>
-      <c r="AN13" s="39">
-        <v>0</v>
-      </c>
-      <c r="AO13" s="39">
-        <v>0</v>
-      </c>
-      <c r="AP13" s="39">
-        <v>0</v>
-      </c>
-      <c r="AQ13" s="40">
+      <c r="AK13" s="32">
+        <v>0</v>
+      </c>
+      <c r="AL13" s="36">
+        <v>0</v>
+      </c>
+      <c r="AM13" s="37">
+        <v>0</v>
+      </c>
+      <c r="AN13" s="37">
+        <v>0</v>
+      </c>
+      <c r="AO13" s="37">
+        <v>0</v>
+      </c>
+      <c r="AP13" s="37">
+        <v>0</v>
+      </c>
+      <c r="AQ13" s="38">
         <v>0</v>
       </c>
     </row>
@@ -1922,26 +1911,9 @@
         <v>9</v>
       </c>
       <c r="L14" s="5"/>
-      <c r="U14" s="27"/>
-      <c r="V14" s="27"/>
-      <c r="W14" s="27"/>
-      <c r="X14" s="27"/>
-      <c r="Y14" s="27"/>
-      <c r="Z14" s="27"/>
-      <c r="AA14" s="27"/>
-      <c r="AB14" s="27"/>
-      <c r="AC14" s="27"/>
-      <c r="AD14" s="27"/>
-      <c r="AE14" s="27"/>
-      <c r="AF14" s="27"/>
-      <c r="AG14" s="27"/>
-      <c r="AH14" s="27"/>
-      <c r="AI14" s="27"/>
-      <c r="AJ14" s="27"/>
-      <c r="AK14" s="28" t="s">
+      <c r="AK14" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="AL14" s="27"/>
     </row>
     <row r="15" spans="1:43" x14ac:dyDescent="0.25">
       <c r="F15" t="s">
@@ -1971,42 +1943,26 @@
       <c r="O15" s="7">
         <v>0</v>
       </c>
-      <c r="U15" s="27"/>
-      <c r="V15" s="27"/>
-      <c r="W15" s="27"/>
-      <c r="X15" s="27"/>
-      <c r="Y15" s="27"/>
-      <c r="Z15" s="27"/>
-      <c r="AA15" s="27"/>
-      <c r="AB15" s="27"/>
-      <c r="AC15" s="27"/>
-      <c r="AD15" s="27"/>
-      <c r="AE15" s="27"/>
-      <c r="AF15" s="27"/>
-      <c r="AG15" s="27"/>
-      <c r="AH15" s="27"/>
-      <c r="AI15" s="27"/>
-      <c r="AJ15" s="27"/>
-      <c r="AK15" s="33" cm="1">
+      <c r="AK15" s="31" cm="1">
         <f t="array" ref="AK15:AQ17">TRANSPOSE($Q23:$S29)-MMULT($K$15:$O$17,TRANSPOSE($K23:$O29))</f>
         <v>0</v>
       </c>
-      <c r="AL15" s="41">
+      <c r="AL15" s="39">
         <v>-2.9999999640040187E-7</v>
       </c>
-      <c r="AM15" s="36">
-        <v>0</v>
-      </c>
-      <c r="AN15" s="36">
-        <v>0</v>
-      </c>
-      <c r="AO15" s="36">
-        <v>0</v>
-      </c>
-      <c r="AP15" s="36">
-        <v>0</v>
-      </c>
-      <c r="AQ15" s="37">
+      <c r="AM15" s="34">
+        <v>0</v>
+      </c>
+      <c r="AN15" s="34">
+        <v>0</v>
+      </c>
+      <c r="AO15" s="34">
+        <v>0</v>
+      </c>
+      <c r="AP15" s="34">
+        <v>0</v>
+      </c>
+      <c r="AQ15" s="35">
         <v>0</v>
       </c>
     </row>
@@ -2038,43 +1994,33 @@
       <c r="O16" s="7">
         <v>0</v>
       </c>
-      <c r="U16" s="28" t="s">
+      <c r="U16" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="V16" s="28"/>
-      <c r="W16" s="28"/>
-      <c r="X16" s="28"/>
-      <c r="Y16" s="28"/>
-      <c r="Z16" s="28"/>
-      <c r="AA16" s="27"/>
-      <c r="AB16" s="27"/>
-      <c r="AC16" s="27"/>
-      <c r="AD16" s="27"/>
-      <c r="AE16" s="27"/>
-      <c r="AF16" s="27"/>
-      <c r="AG16" s="27"/>
-      <c r="AH16" s="27"/>
-      <c r="AI16" s="27"/>
-      <c r="AJ16" s="27"/>
+      <c r="V16" s="5"/>
+      <c r="W16" s="5"/>
+      <c r="X16" s="5"/>
+      <c r="Y16" s="5"/>
+      <c r="Z16" s="5"/>
       <c r="AK16" s="25">
         <v>0</v>
       </c>
-      <c r="AL16" s="30">
-        <v>0</v>
-      </c>
-      <c r="AM16" s="27">
-        <v>0</v>
-      </c>
-      <c r="AN16" s="27">
-        <v>0</v>
-      </c>
-      <c r="AO16" s="27">
-        <v>0</v>
-      </c>
-      <c r="AP16" s="27">
-        <v>0</v>
-      </c>
-      <c r="AQ16" s="42">
+      <c r="AL16" s="28">
+        <v>0</v>
+      </c>
+      <c r="AM16">
+        <v>0</v>
+      </c>
+      <c r="AN16">
+        <v>0</v>
+      </c>
+      <c r="AO16">
+        <v>0</v>
+      </c>
+      <c r="AP16">
+        <v>0</v>
+      </c>
+      <c r="AQ16" s="40">
         <v>0</v>
       </c>
     </row>
@@ -2106,44 +2052,34 @@
       <c r="O17" s="7">
         <v>1</v>
       </c>
-      <c r="U17" s="31">
+      <c r="U17" s="29">
         <f>SUM(Q41:S47)</f>
         <v>417.33333340000001</v>
       </c>
-      <c r="AA17" s="27"/>
-      <c r="AB17" s="27"/>
-      <c r="AC17" s="27"/>
-      <c r="AD17" s="27"/>
-      <c r="AE17" s="27"/>
-      <c r="AF17" s="27"/>
-      <c r="AG17" s="27"/>
-      <c r="AH17" s="27"/>
-      <c r="AI17" s="27"/>
-      <c r="AJ17" s="27"/>
       <c r="AK17" s="24">
         <v>0</v>
       </c>
-      <c r="AL17" s="43">
-        <v>0</v>
-      </c>
-      <c r="AM17" s="39">
-        <v>0</v>
-      </c>
-      <c r="AN17" s="39">
-        <v>0</v>
-      </c>
-      <c r="AO17" s="39">
-        <v>0</v>
-      </c>
-      <c r="AP17" s="39">
-        <v>0</v>
-      </c>
-      <c r="AQ17" s="40">
+      <c r="AL17" s="41">
+        <v>0</v>
+      </c>
+      <c r="AM17" s="37">
+        <v>0</v>
+      </c>
+      <c r="AN17" s="37">
+        <v>0</v>
+      </c>
+      <c r="AO17" s="37">
+        <v>0</v>
+      </c>
+      <c r="AP17" s="37">
+        <v>0</v>
+      </c>
+      <c r="AQ17" s="38">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="Q18" s="45" t="s">
+      <c r="Q18" s="43" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2154,7 +2090,7 @@
       <c r="I19" t="s">
         <v>11</v>
       </c>
-      <c r="K19" s="45" t="s">
+      <c r="K19" s="43" t="s">
         <v>25</v>
       </c>
       <c r="Q19" s="7">
@@ -2195,10 +2131,10 @@
       <c r="O20" s="7">
         <v>0</v>
       </c>
-      <c r="U20" s="44">
+      <c r="U20" s="42">
         <v>50</v>
       </c>
-      <c r="W20" s="46">
+      <c r="W20" s="44">
         <f>SUM(K32:M38)-U20</f>
         <v>-4.9999997031591192E-8</v>
       </c>
@@ -2242,7 +2178,6 @@
       <c r="O23" s="26">
         <v>0</v>
       </c>
-      <c r="P23" s="27"/>
       <c r="Q23" s="26">
         <v>0</v>
       </c>
@@ -2281,7 +2216,6 @@
       <c r="O24" s="26">
         <v>0</v>
       </c>
-      <c r="P24" s="27"/>
       <c r="Q24" s="26">
         <v>43.333333000000003</v>
       </c>
@@ -2291,7 +2225,7 @@
       <c r="S24" s="26">
         <v>26.666667</v>
       </c>
-      <c r="U24" s="44">
+      <c r="U24" s="42">
         <v>0</v>
       </c>
     </row>
@@ -2320,7 +2254,6 @@
       <c r="O25" s="26">
         <v>0</v>
       </c>
-      <c r="P25" s="27"/>
       <c r="Q25" s="26">
         <v>30</v>
       </c>
@@ -2330,7 +2263,7 @@
       <c r="S25" s="26">
         <v>0</v>
       </c>
-      <c r="U25" s="44">
+      <c r="U25" s="42">
         <v>0</v>
       </c>
     </row>
@@ -2359,7 +2292,6 @@
       <c r="O26" s="26">
         <v>0</v>
       </c>
-      <c r="P26" s="27"/>
       <c r="Q26" s="26">
         <v>40</v>
       </c>
@@ -2395,7 +2327,6 @@
       <c r="O27" s="26">
         <v>0</v>
       </c>
-      <c r="P27" s="27"/>
       <c r="Q27" s="26">
         <v>0</v>
       </c>
@@ -2434,7 +2365,6 @@
       <c r="O28" s="26">
         <v>0</v>
       </c>
-      <c r="P28" s="27"/>
       <c r="Q28" s="26">
         <v>150</v>
       </c>
@@ -2444,7 +2374,7 @@
       <c r="S28" s="26">
         <v>0</v>
       </c>
-      <c r="U28" s="44">
+      <c r="U28" s="42">
         <v>0</v>
       </c>
     </row>
@@ -2473,7 +2403,6 @@
       <c r="O29" s="26">
         <v>0</v>
       </c>
-      <c r="P29" s="27"/>
       <c r="Q29" s="26">
         <v>150</v>
       </c>
@@ -2483,7 +2412,7 @@
       <c r="S29" s="26">
         <v>0</v>
       </c>
-      <c r="U29" s="44">
+      <c r="U29" s="42">
         <v>0</v>
       </c>
     </row>
@@ -2502,20 +2431,20 @@
       <c r="C32" t="s">
         <v>70</v>
       </c>
-      <c r="K32" s="29" cm="1">
+      <c r="K32" s="27" cm="1">
         <f t="array" ref="K32:O38">$K23:$O29*$K$20:$O$20</f>
         <v>0</v>
       </c>
-      <c r="L32" s="29">
-        <v>0</v>
-      </c>
-      <c r="M32" s="29">
-        <v>0</v>
-      </c>
-      <c r="N32" s="29">
-        <v>0</v>
-      </c>
-      <c r="O32" s="29">
+      <c r="L32" s="27">
+        <v>0</v>
+      </c>
+      <c r="M32" s="27">
+        <v>0</v>
+      </c>
+      <c r="N32" s="27">
+        <v>0</v>
+      </c>
+      <c r="O32" s="27">
         <v>0</v>
       </c>
     </row>
@@ -2529,19 +2458,19 @@
       <c r="C33" t="s">
         <v>70</v>
       </c>
-      <c r="K33" s="29">
+      <c r="K33" s="27">
         <v>4.9999999500000003</v>
       </c>
-      <c r="L33" s="29">
-        <v>0</v>
-      </c>
-      <c r="M33" s="29">
-        <v>0</v>
-      </c>
-      <c r="N33" s="29">
+      <c r="L33" s="27">
+        <v>0</v>
+      </c>
+      <c r="M33" s="27">
+        <v>0</v>
+      </c>
+      <c r="N33" s="27">
         <v>80</v>
       </c>
-      <c r="O33" s="29">
+      <c r="O33" s="27">
         <v>0</v>
       </c>
     </row>
@@ -2555,19 +2484,19 @@
       <c r="C34" t="s">
         <v>70</v>
       </c>
-      <c r="K34" s="29">
+      <c r="K34" s="27">
         <v>45</v>
       </c>
-      <c r="L34" s="29">
-        <v>0</v>
-      </c>
-      <c r="M34" s="29">
-        <v>0</v>
-      </c>
-      <c r="N34" s="29">
-        <v>0</v>
-      </c>
-      <c r="O34" s="29">
+      <c r="L34" s="27">
+        <v>0</v>
+      </c>
+      <c r="M34" s="27">
+        <v>0</v>
+      </c>
+      <c r="N34" s="27">
+        <v>0</v>
+      </c>
+      <c r="O34" s="27">
         <v>0</v>
       </c>
     </row>
@@ -2581,19 +2510,19 @@
       <c r="C35" t="s">
         <v>70</v>
       </c>
-      <c r="K35" s="29">
-        <v>0</v>
-      </c>
-      <c r="L35" s="29">
-        <v>0</v>
-      </c>
-      <c r="M35" s="29">
-        <v>0</v>
-      </c>
-      <c r="N35" s="29">
+      <c r="K35" s="27">
+        <v>0</v>
+      </c>
+      <c r="L35" s="27">
+        <v>0</v>
+      </c>
+      <c r="M35" s="27">
+        <v>0</v>
+      </c>
+      <c r="N35" s="27">
         <v>80</v>
       </c>
-      <c r="O35" s="29">
+      <c r="O35" s="27">
         <v>0</v>
       </c>
     </row>
@@ -2607,19 +2536,19 @@
       <c r="C36" t="s">
         <v>70</v>
       </c>
-      <c r="K36" s="29">
-        <v>0</v>
-      </c>
-      <c r="L36" s="29">
-        <v>0</v>
-      </c>
-      <c r="M36" s="29">
-        <v>0</v>
-      </c>
-      <c r="N36" s="29">
-        <v>0</v>
-      </c>
-      <c r="O36" s="29">
+      <c r="K36" s="27">
+        <v>0</v>
+      </c>
+      <c r="L36" s="27">
+        <v>0</v>
+      </c>
+      <c r="M36" s="27">
+        <v>0</v>
+      </c>
+      <c r="N36" s="27">
+        <v>0</v>
+      </c>
+      <c r="O36" s="27">
         <v>0</v>
       </c>
     </row>
@@ -2633,19 +2562,19 @@
       <c r="C37" t="s">
         <v>57</v>
       </c>
-      <c r="K37" s="29">
-        <v>0</v>
-      </c>
-      <c r="L37" s="29">
-        <v>0</v>
-      </c>
-      <c r="M37" s="29">
-        <v>0</v>
-      </c>
-      <c r="N37" s="29">
+      <c r="K37" s="27">
+        <v>0</v>
+      </c>
+      <c r="L37" s="27">
+        <v>0</v>
+      </c>
+      <c r="M37" s="27">
+        <v>0</v>
+      </c>
+      <c r="N37" s="27">
         <v>300</v>
       </c>
-      <c r="O37" s="29">
+      <c r="O37" s="27">
         <v>0</v>
       </c>
     </row>
@@ -2659,45 +2588,27 @@
       <c r="C38" t="s">
         <v>57</v>
       </c>
-      <c r="K38" s="29">
-        <v>0</v>
-      </c>
-      <c r="L38" s="29">
-        <v>0</v>
-      </c>
-      <c r="M38" s="29">
-        <v>0</v>
-      </c>
-      <c r="N38" s="29">
+      <c r="K38" s="27">
+        <v>0</v>
+      </c>
+      <c r="L38" s="27">
+        <v>0</v>
+      </c>
+      <c r="M38" s="27">
+        <v>0</v>
+      </c>
+      <c r="N38" s="27">
         <v>300</v>
       </c>
-      <c r="O38" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="K39" s="27"/>
-      <c r="L39" s="27"/>
-      <c r="M39" s="27"/>
-      <c r="N39" s="27"/>
-      <c r="O39" s="27"/>
-      <c r="P39" s="27"/>
-      <c r="Q39" s="27"/>
-      <c r="R39" s="27"/>
-      <c r="S39" s="27"/>
+      <c r="O38" s="27">
+        <v>0</v>
+      </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="K40" s="27"/>
-      <c r="L40" s="27"/>
-      <c r="M40" s="27"/>
-      <c r="N40" s="27"/>
-      <c r="O40" s="27"/>
-      <c r="P40" s="27"/>
-      <c r="Q40" s="28" t="s">
+      <c r="Q40" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="R40" s="28"/>
-      <c r="S40" s="27"/>
+      <c r="R40" s="5"/>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
@@ -2709,20 +2620,14 @@
       <c r="C41" t="s">
         <v>70</v>
       </c>
-      <c r="K41" s="27"/>
-      <c r="L41" s="27"/>
-      <c r="M41" s="27"/>
-      <c r="N41" s="27"/>
-      <c r="O41" s="27"/>
-      <c r="P41" s="27"/>
-      <c r="Q41" s="29" cm="1">
+      <c r="Q41" s="27" cm="1">
         <f t="array" ref="Q41:S47">$Q23:$S29*$Q$19:$S$19</f>
         <v>0</v>
       </c>
-      <c r="R41" s="29">
+      <c r="R41" s="27">
         <v>15</v>
       </c>
-      <c r="S41" s="29">
+      <c r="S41" s="27">
         <v>0</v>
       </c>
     </row>
@@ -2736,19 +2641,13 @@
       <c r="C42" t="s">
         <v>70</v>
       </c>
-      <c r="K42" s="27"/>
-      <c r="L42" s="27"/>
-      <c r="M42" s="27"/>
-      <c r="N42" s="27"/>
-      <c r="O42" s="27"/>
-      <c r="P42" s="27"/>
-      <c r="Q42" s="29">
+      <c r="Q42" s="27">
         <v>34.666666400000004</v>
       </c>
-      <c r="R42" s="29">
-        <v>0</v>
-      </c>
-      <c r="S42" s="29">
+      <c r="R42" s="27">
+        <v>0</v>
+      </c>
+      <c r="S42" s="27">
         <v>26.666667</v>
       </c>
     </row>
@@ -2762,19 +2661,13 @@
       <c r="C43" t="s">
         <v>70</v>
       </c>
-      <c r="K43" s="27"/>
-      <c r="L43" s="27"/>
-      <c r="M43" s="27"/>
-      <c r="N43" s="27"/>
-      <c r="O43" s="27"/>
-      <c r="P43" s="27"/>
-      <c r="Q43" s="29">
+      <c r="Q43" s="27">
         <v>24</v>
       </c>
-      <c r="R43" s="29">
-        <v>0</v>
-      </c>
-      <c r="S43" s="29">
+      <c r="R43" s="27">
+        <v>0</v>
+      </c>
+      <c r="S43" s="27">
         <v>0</v>
       </c>
     </row>
@@ -2788,19 +2681,13 @@
       <c r="C44" t="s">
         <v>70</v>
       </c>
-      <c r="K44" s="27"/>
-      <c r="L44" s="27"/>
-      <c r="M44" s="27"/>
-      <c r="N44" s="27"/>
-      <c r="O44" s="27"/>
-      <c r="P44" s="27"/>
-      <c r="Q44" s="29">
+      <c r="Q44" s="27">
         <v>32</v>
       </c>
-      <c r="R44" s="29">
+      <c r="R44" s="27">
         <v>15</v>
       </c>
-      <c r="S44" s="29">
+      <c r="S44" s="27">
         <v>0</v>
       </c>
     </row>
@@ -2814,19 +2701,13 @@
       <c r="C45" t="s">
         <v>70</v>
       </c>
-      <c r="K45" s="27"/>
-      <c r="L45" s="27"/>
-      <c r="M45" s="27"/>
-      <c r="N45" s="27"/>
-      <c r="O45" s="27"/>
-      <c r="P45" s="27"/>
-      <c r="Q45" s="29">
-        <v>0</v>
-      </c>
-      <c r="R45" s="29">
+      <c r="Q45" s="27">
+        <v>0</v>
+      </c>
+      <c r="R45" s="27">
         <v>15</v>
       </c>
-      <c r="S45" s="29">
+      <c r="S45" s="27">
         <v>0</v>
       </c>
     </row>
@@ -2840,19 +2721,13 @@
       <c r="C46" t="s">
         <v>57</v>
       </c>
-      <c r="K46" s="27"/>
-      <c r="L46" s="27"/>
-      <c r="M46" s="27"/>
-      <c r="N46" s="27"/>
-      <c r="O46" s="27"/>
-      <c r="P46" s="27"/>
-      <c r="Q46" s="29">
+      <c r="Q46" s="27">
         <v>120</v>
       </c>
-      <c r="R46" s="29">
+      <c r="R46" s="27">
         <v>7.5</v>
       </c>
-      <c r="S46" s="29">
+      <c r="S46" s="27">
         <v>0</v>
       </c>
     </row>
@@ -2866,32 +2741,15 @@
       <c r="C47" t="s">
         <v>57</v>
       </c>
-      <c r="K47" s="27"/>
-      <c r="L47" s="27"/>
-      <c r="M47" s="27"/>
-      <c r="N47" s="27"/>
-      <c r="O47" s="27"/>
-      <c r="P47" s="27"/>
-      <c r="Q47" s="29">
+      <c r="Q47" s="27">
         <v>120</v>
       </c>
-      <c r="R47" s="29">
+      <c r="R47" s="27">
         <v>7.5</v>
       </c>
-      <c r="S47" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="K48" s="27"/>
-      <c r="L48" s="27"/>
-      <c r="M48" s="27"/>
-      <c r="N48" s="27"/>
-      <c r="O48" s="27"/>
-      <c r="P48" s="27"/>
-      <c r="Q48" s="27"/>
-      <c r="R48" s="27"/>
-      <c r="S48" s="27"/>
+      <c r="S47" s="27">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2918,22 +2776,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="50" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="53" t="s">
+      <c r="C1" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="53" t="s">
+      <c r="D1" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="53" t="s">
+      <c r="E1" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="53" t="s">
+      <c r="F1" s="49" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>